<commit_message>
Actualización: Base de datos y plantilla Word actualizadas
</commit_message>
<xml_diff>
--- a/PLANTILLA 29D AUDITORIA.xlsx
+++ b/PLANTILLA 29D AUDITORIA.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/67fdac007ebf7936/Attachments/Documentos/Interfaces de phyton/oficios automatizados Lap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sup11\Ghernandez0205\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{9D1007BE-26E8-445C-9278-2F1AA212750E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF89FA67-F409-4F6C-8681-DC63879E7B6A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00656E7F-8355-4324-BD4F-5671BEFDB41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUP 29D" sheetId="13" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SUP 29D'!$A$1:$G$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SUP 29D'!$A$1:$G$38</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="157">
   <si>
     <t>NIVEL EDUCATIVO</t>
   </si>
@@ -428,15 +428,6 @@
   </si>
   <si>
     <t>RASD8212191F8</t>
-  </si>
-  <si>
-    <t>SOSA</t>
-  </si>
-  <si>
-    <t>JOSE GUILLERMO</t>
-  </si>
-  <si>
-    <t>RASG660608VB3</t>
   </si>
   <si>
     <t>RIOS</t>
@@ -953,24 +944,24 @@
     <tabColor theme="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="82" zoomScaleNormal="95" zoomScaleSheetLayoutView="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScale="82" zoomScaleNormal="95" zoomScaleSheetLayoutView="82" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G44"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="11.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="22.28515625" customWidth="1"/>
+    <col min="6" max="7" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="50.45" customHeight="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="50.4" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1004,16 +995,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" ht="18.75" customHeight="1">
@@ -1188,7 +1179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="28.15" customHeight="1">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="28.2" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1280,7 +1271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="22.9" customHeight="1">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="22.95" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1331,16 +1322,16 @@
         <v>0</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" ht="18.75" customHeight="1">
@@ -1552,13 +1543,13 @@
         <v>78</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="4" customFormat="1" ht="18.75" customHeight="1">
@@ -1802,77 +1793,68 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A39" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="9">
-        <v>0</v>
-      </c>
+    <row r="39" spans="1:7">
       <c r="D39" s="10" t="s">
         <v>47</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="D40" s="10" t="s">
-        <v>47</v>
+        <v>148</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="21.6" customHeight="1">
       <c r="D41" s="10" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="21.6" customHeight="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="D42" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.6" customHeight="1">
       <c r="D43" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>138</v>
+        <v>70</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>139</v>
@@ -1881,23 +1863,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.6" customHeight="1">
-      <c r="D44" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:G44">
-    <sortCondition ref="D1:D44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:G43">
+    <sortCondition ref="D1:D43"/>
   </sortState>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.15748031496062992" right="3.937007874015748E-2" top="0.23622047244094491" bottom="0.35433070866141736" header="0.19685039370078741" footer="0.31496062992125984"/>

</xml_diff>